<commit_message>
Added 2.205 Campaign Files
</commit_message>
<xml_diff>
--- a/BalanceInfo/Core Comparison/HWR Core Comparison_2.3 build 8 WIP.xlsx
+++ b/BalanceInfo/Core Comparison/HWR Core Comparison_2.3 build 8 WIP.xlsx
@@ -300,7 +300,7 @@
     <t>Stats are from Homeworld Remastered as of:</t>
   </si>
   <si>
-    <t>2.3 Players Patch build 8 WIP</t>
+    <t>2.3 Players Patch build 8</t>
   </si>
 </sst>
 </file>
@@ -759,7 +759,7 @@
         <v>88</v>
       </c>
       <c r="B5" s="31">
-        <v>43311</v>
+        <v>43316</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>89</v>

</xml_diff>